<commit_message>
add relation values to input for egasoline
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/egasoline/Model_Data_Base_egasoline_4_InOutputs.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/egasoline/Model_Data_Base_egasoline_4_InOutputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/egasoline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\egasoline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{B63BCB0A-9012-4F55-92B6-F45564B797E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8929016F-90E9-462D-9347-382C38A696EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505DA5C3-9445-46B4-88E6-67A195B16402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1560" yWindow="-19440" windowWidth="38700" windowHeight="15315" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="128">
   <si>
     <t>Unit</t>
   </si>
@@ -343,15 +343,9 @@
     <t>heat_high</t>
   </si>
   <si>
-    <t>heat_split</t>
-  </si>
-  <si>
     <t>Auxilliary</t>
   </si>
   <si>
-    <t>internal_heat</t>
-  </si>
-  <si>
     <t>Input3</t>
   </si>
   <si>
@@ -455,6 +449,15 @@
   </si>
   <si>
     <t>gasoline_st</t>
+  </si>
+  <si>
+    <t>power_steam</t>
+  </si>
+  <si>
+    <t>co2_source</t>
+  </si>
+  <si>
+    <t>heat_recovery</t>
   </si>
 </sst>
 </file>
@@ -564,6 +567,621 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -648,621 +1266,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1311,26 +1314,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q12" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:Q12" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}" name="Table5" displayName="Table5" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="0" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:Q14" xr:uid="{C1664CC4-80CB-414D-BAFE-57FF9635D79F}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{2BE3E317-773B-4E82-9035-69A43C6CB21B}" name="Unit" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{22613EE0-390D-4B04-9A9B-6D5554D1C8ED}" name="Object_type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{54CD83B6-B63A-4ABD-99BD-9ED391BFB078}" name="Input1" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{F183F72C-A42E-4046-9CA2-B23C4DD3765C}" name="Input2" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{CA468CF3-FA3A-4DED-8C1A-ED8385FD2167}" name="Input3" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{6C9174ED-453E-45B1-B2C9-DC69B7CB535A}" name="Input4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{513A63E4-7BE3-4AF5-AC5E-11EB4AF0D7AD}" name="Output1" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{4623E738-60A2-497B-BD61-91A608129A61}" name="Output2" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{5596B30B-5CDD-4E38-8C15-9C5F774E9B1F}" name="Output3" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{CD6FCAF1-2543-4CF8-99F5-E24DBA2DEDC0}" name="Output4" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{88F2DAC4-E2C3-4C34-B709-2523E8BE5B1F}" name="Relation_In1_In2" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{3C190E97-FD9A-4F36-8EBF-717B1ECA00B1}" name="Relation_In1_In3" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{043147D8-AE82-457E-8F19-EB4AE9D43B9E}" name="Relation_In1_In4" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{A190E492-7FDF-403D-B8AF-17448A48E47F}" name="Relation_In1_Out1" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{26E8D274-C985-4E20-8920-2BAC0A372552}" name="Relation_Out1_Out2" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{4E0BCAE8-11F8-4D98-AECC-86C8A3C2B5C1}" name="Relation_Out1_Out3" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{3C0369D5-4DD0-4B4B-9480-0C4665C0BC59}" name="Relation_Out1_Out4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1346,7 +1349,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="22"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -1365,7 +1368,7 @@
     <tableColumn id="21" xr3:uid="{EC2CC790-C17D-4744-A981-3984808E5B33}" name="vom_cost_Input2"/>
     <tableColumn id="24" xr3:uid="{41B338E4-2058-41E9-8000-97D77450FBC3}" name="vom_cost_Output1"/>
     <tableColumn id="25" xr3:uid="{DDAFCF0A-1EF1-4B7B-9742-01F9FA7A22E5}" name="vom_cost_Output2"/>
-    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{79DE3A19-CED6-47DE-AEF5-F6BB2D320F24}" name="connection_investment_tech_lifetime" dataDxfId="21"/>
     <tableColumn id="30" xr3:uid="{09434E4A-7BF5-4547-9708-EA3F0F7ADC8E}" name="initial_connections_invested_available"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1376,7 +1379,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:K5" totalsRowShown="0">
   <autoFilter ref="A1:K5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="20">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{8C29206C-8DC6-44DB-A8D1-3D5625C277AD}" name="Object_type"/>
@@ -1730,7 +1733,7 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -1739,16 +1742,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J1" t="s">
         <v>64</v>
@@ -1793,7 +1796,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -1806,7 +1809,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -1860,7 +1863,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>42</v>
@@ -1871,10 +1874,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
         <v>78</v>
@@ -1900,10 +1903,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -1916,10 +1919,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
@@ -1932,13 +1935,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -1972,10 +1975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CABA7C5-6230-4207-9D35-0A95D86E66AC}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1999,10 +2002,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -2011,31 +2014,31 @@
         <v>4</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -2065,7 +2068,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>62</v>
@@ -2090,7 +2093,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -2189,35 +2192,41 @@
         <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4">
+        <v>161.1904761904762</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="N7" s="4">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1.4999999999999998</v>
+      </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>78</v>
@@ -2225,18 +2234,30 @@
       <c r="D8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="G8" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="K8" s="3">
+        <v>2.8982576753129519</v>
+      </c>
+      <c r="L8" s="3">
+        <v>12.285714285714285</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3.0714285714285712</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.86</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -2249,7 +2270,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>75</v>
@@ -2263,12 +2284,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4">
-        <v>7.2437800000000002E-4</v>
+        <v>9.8530247749999979E-4</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4">
-        <v>0.99</v>
+        <v>1.0101010101010102</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
@@ -2276,27 +2297,36 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2313,65 +2343,108 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="J12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="6">
+        <v>42.75</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1.6132075471698113</v>
+      </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="N12" s="6">
+        <v>1.6285714285714283</v>
+      </c>
+      <c r="O12" s="6">
+        <v>6.7340067340067344</v>
+      </c>
+      <c r="P12" s="6">
+        <v>5.5096418732782366</v>
+      </c>
       <c r="Q12" s="6"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
+        <v>1.1883541295306002</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6">
         <v>1</v>
       </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2386,7 +2459,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B13 B1:B12</xm:sqref>
+          <xm:sqref>B1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2398,7 +2471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2628,22 +2701,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" t="s">
-        <v>125</v>
-      </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
@@ -2795,10 +2868,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2944,32 +3017,32 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>